<commit_message>
Edits excel.php, task pdf
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -15,7 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+  <si>
+    <t>Результаты расчета</t>
+  </si>
   <si>
     <t>Тип ТС и категория:</t>
   </si>
@@ -23,7 +26,7 @@
     <t>ТС категория А М</t>
   </si>
   <si>
-    <t>Мощность двигателя:</t>
+    <t>Мощность двигателя (лошадиные силы):</t>
   </si>
   <si>
     <t>до 50 включительно</t>
@@ -41,7 +44,7 @@
     <t>Ограниченое количество лиц допущеных к управлению ТС</t>
   </si>
   <si>
-    <t>Период страховки (для иносранных агентов):</t>
+    <t>Период страховки (для иностранных агентов):</t>
   </si>
   <si>
     <t>от 5 до 15 дней</t>
@@ -53,22 +56,22 @@
     <t>m</t>
   </si>
   <si>
-    <t>Возраст водителя:</t>
+    <t>Возраст водителя (период в годовом выражение):</t>
   </si>
   <si>
     <t>16-21</t>
   </si>
   <si>
-    <t>Водительский стаж:</t>
-  </si>
-  <si>
-    <t>Является ли иностранным агентом:</t>
+    <t>Водительский стаж (количество полных лет):</t>
+  </si>
+  <si>
+    <t>ТС зарегестрировано в иностраном государстве:</t>
   </si>
   <si>
     <t>да</t>
   </si>
   <si>
-    <t>Юр. лицо или физ. лицо:</t>
+    <t>Юридическая форма:</t>
   </si>
   <si>
     <t>физ. лицо</t>
@@ -94,7 +97,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -102,6 +105,15 @@
       <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -116,18 +128,74 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,116 +496,126 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1:B13"/>
+      <selection activeCell="A1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="60" customWidth="true" style="0"/>
+    <col min="2" max="2" width="60" customWidth="true" style="0"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
+      <c r="B9" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="3" t="s">
         <v>23</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>